<commit_message>
Update Peer Review Log (Phase 1)_v2.xlsx
</commit_message>
<xml_diff>
--- a/Week 5 Phase I/Peer Review Log (Phase 1)_v2.xlsx
+++ b/Week 5 Phase I/Peer Review Log (Phase 1)_v2.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A91DD368-F21F-4B5F-B3DC-A2B1C3BE37F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69DD5F8-F0AC-41FD-9469-75B5801F7A4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,35 +167,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,33 +480,33 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K4:K7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -526,98 +526,98 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>43875</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>